<commit_message>
feat: parse class group sessions (#128)
</commit_message>
<xml_diff>
--- a/backend/internal/servers/apiserver/common/batch_file_well_formatted.xlsx
+++ b/backend/internal/servers/apiserver/common/batch_file_well_formatted.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">Class Group: A32</t>
   </si>
   <si>
-    <t xml:space="preserve">Day-Time: Tue  1130 To: 1220 Wk2-13</t>
+    <t xml:space="preserve">Day-Time: Tue  1130 To: 1220 Wk2,4,6,8,10,12</t>
   </si>
   <si>
     <t xml:space="preserve">Venue: TR+37 NORTH,NS2-05-30</t>
@@ -603,11 +603,11 @@
   </sheetPr>
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>

</xml_diff>

<commit_message>
feat: implement class managers table (#169)
</commit_message>
<xml_diff>
--- a/backend/internal/servers/apiserver/common/batch_file_well_formatted.xlsx
+++ b/backend/internal/servers/apiserver/common/batch_file_well_formatted.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="160">
-  <si>
-    <t xml:space="preserve">Class Attendance List: 2022, 2  Date: 15-JUN-2023 13:01</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="169">
+  <si>
+    <t xml:space="preserve">Class Attendance List: 2023, 2  Date: 15-JUN-2023 13:01</t>
   </si>
   <si>
     <t xml:space="preserve">Programme: CSC  Full-Time</t>
@@ -55,399 +55,423 @@
     <t xml:space="preserve">Prog/ Yr/ Student Type/ Course Type/ Nationality/ VMS Acc</t>
   </si>
   <si>
+    <t xml:space="preserve">HAR JING DARYL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSC3 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARJ0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUA XIN YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUX6789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOH KAI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSAI3 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOHK4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOH WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOHW4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOH KAI XUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOHK2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOH MEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOHM2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE HYUNSUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEH9898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE JIA YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEJ5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE WEI XUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEW5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE XIN YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEX5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIM HUI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMH5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIM WEI CHEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMW1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIM XIN TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMX5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG JIA MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGJI9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG KAI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGKA9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG LI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSC4 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGLI9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGUYEN HOANG NHAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGUY0012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONG WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSAI4 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONGW3210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONG WEI XUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONGW3211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN JIA LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANJ4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN KAI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANK4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANW5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAY HUI MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAYH7654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAY LI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAYL7654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONG HUI MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONH7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONG MEI CHEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONM7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAP KAI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAPK9087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAP WEN LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAPW9087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Group: A26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day-Time: Mon  0130 To: 0220 Wk2-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venue: TR+19 NORTH,NS4-05-97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENJAMIN SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENST129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUA JIA LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUJ6788</t>
+  </si>
+  <si>
     <t xml:space="preserve">CHUA LI TING</t>
   </si>
   <si>
-    <t xml:space="preserve">CSC3 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG</t>
+    <t xml:space="preserve">REP3 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">CHUL6789</t>
   </si>
   <si>
-    <t xml:space="preserve">CHUA XIN YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHUX6789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOH KAI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSAI3 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOHK4567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOH WEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOHW4567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOH KAI XUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOHK2345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOH MEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOHM2345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE HYUNSUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEH9898</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE JIA YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEJ5432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE WEI XUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEW5432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE XIN YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEX5432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIM HUI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIMH5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIM WEI CHEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIMW1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIM XIN TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIMX5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG JIA MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGJI9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG KAI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGKA9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG LI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSC4 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGLI9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGUYEN HOANG NHAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGUY0012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONG WEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSAI4 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG PR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONGW3210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONG WEI XUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONGW3211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN JIA LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TANJ4321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN KAI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TANK4321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN WEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TANW5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAY HUI MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAYH7654</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAY LI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAYL7654</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONG HUI MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONH7890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONG MEI CHEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONM7890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAP KAI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAPK9087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAP WEN LI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAPW9087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class Group: A26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day-Time: Mon  0130 To: 0220 Wk2-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venue: TR+19 NORTH,NS4-05-97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENJAMIN SANTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENST129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHUA JIA LING</t>
+    <t xml:space="preserve">CHUA WEN LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUW6789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOH KAI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOHK4568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOH XIN TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACDA3 FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOHX4567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHN SMITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12115452G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOSEPHINE KURNIAWAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOSEPHI09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOH HUI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOHU2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOH LI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KOHL2345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE KAI WEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEEK5432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIM LI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIML5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIM MEI CHEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMM5678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAKAMURA HARUKI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T67516625Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGWL9876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONG HUI MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONGH3210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONG XIN YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONGX3210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHAN HOANG TRAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHHOANG1827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN KAI XUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANK4322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN XIN YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANX4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAY LI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAYL7655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONG JIA MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONJ7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONG WEI XUAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WONW7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAP MEI TING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAPM9087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAP WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAPW9088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Group: A32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day-Time: Tue  1130 To: 1220 Wk2,4,6,8,10,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venue: TR+37 NORTH,NS2-05-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARJUN PATEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATELAR14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUA JIA MIN</t>
   </si>
   <si>
     <t xml:space="preserve">CHUJ6789</t>
   </si>
   <si>
-    <t xml:space="preserve">REP3 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHUA WEN LI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHUW6789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOH KAI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOH XIN TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACDA3 FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOHX4567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOHN SMITH</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12115452G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSEPHINE KURNIAWAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOSEPHI09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOH HUI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOHU2345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOH LI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOHL2345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE KAI WEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEEK5432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIM LI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIML5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIM MEI CHEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIMM5678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAKAMURA HARUKI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T67516625Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG WEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGWL9876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONG HUI MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONGH3210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONG XIN YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONGX3210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHAN HOANG TRAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHHOANG1827</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN KAI XUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN XIN YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TANX4321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAY LI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONG JIA MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONJ7890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONG WEI XUAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WONW7890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAP MEI TING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAPM9087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAP WEI LING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAPW9088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class Group: A32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day-Time: Tue  1130 To: 1220 Wk2,4,6,8,10,12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venue: TR+37 NORTH,NS2-05-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARJUN PATEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PATELAR14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHUA JIA MIN</t>
+    <t xml:space="preserve">GOHK4569</t>
   </si>
   <si>
     <t xml:space="preserve">KOH MEI CHEN</t>
   </si>
   <si>
+    <t xml:space="preserve">KOHM2346</t>
+  </si>
+  <si>
     <t xml:space="preserve">LEE HUI TING</t>
   </si>
   <si>
@@ -464,6 +488,9 @@
   </si>
   <si>
     <t xml:space="preserve">LIM HUI MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMH5679</t>
   </si>
   <si>
     <t xml:space="preserve">NG KAI LING</t>
@@ -603,11 +630,11 @@
   </sheetPr>
   <dimension ref="A1:F1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F81" activeCellId="0" sqref="F81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1307,19 +1334,19 @@
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1327,7 +1354,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>19</v>
@@ -1339,7 +1366,7 @@
         <v>31</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,7 +1374,7 @@
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>19</v>
@@ -1359,7 +1386,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1367,10 +1394,10 @@
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
@@ -1379,7 +1406,7 @@
         <v>14</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1387,19 +1414,19 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1407,7 +1434,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>12</v>
@@ -1416,10 +1443,10 @@
         <v>13</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1427,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>12</v>
@@ -1439,7 +1466,7 @@
         <v>14</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1447,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>12</v>
@@ -1459,7 +1486,7 @@
         <v>14</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1467,7 +1494,7 @@
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>12</v>
@@ -1479,7 +1506,7 @@
         <v>31</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1487,7 +1514,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>12</v>
@@ -1499,7 +1526,7 @@
         <v>14</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1507,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>12</v>
@@ -1519,7 +1546,7 @@
         <v>14</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1527,19 +1554,19 @@
         <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1547,7 +1574,7 @@
         <v>15</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>48</v>
@@ -1559,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1567,7 +1594,7 @@
         <v>16</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>12</v>
@@ -1579,7 +1606,7 @@
         <v>14</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1587,7 +1614,7 @@
         <v>17</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>12</v>
@@ -1599,7 +1626,7 @@
         <v>55</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1607,7 +1634,7 @@
         <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>12</v>
@@ -1619,7 +1646,7 @@
         <v>51</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1627,7 +1654,7 @@
         <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>12</v>
@@ -1639,7 +1666,7 @@
         <v>14</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1647,7 +1674,7 @@
         <v>20</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>48</v>
@@ -1659,7 +1686,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1667,7 +1694,7 @@
         <v>21</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>12</v>
@@ -1679,7 +1706,7 @@
         <v>14</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1687,7 +1714,7 @@
         <v>22</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>19</v>
@@ -1699,7 +1726,7 @@
         <v>14</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1707,7 +1734,7 @@
         <v>23</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
@@ -1719,7 +1746,7 @@
         <v>14</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1727,7 +1754,7 @@
         <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -1739,7 +1766,7 @@
         <v>31</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1747,7 +1774,7 @@
         <v>25</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>12</v>
@@ -1759,23 +1786,23 @@
         <v>14</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1795,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>19</v>
@@ -1804,10 +1831,10 @@
         <v>13</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1815,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>19</v>
@@ -1827,7 +1854,7 @@
         <v>14</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1835,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>12</v>
@@ -1847,7 +1874,7 @@
         <v>14</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1855,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>19</v>
@@ -1867,7 +1894,7 @@
         <v>14</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1875,7 +1902,7 @@
         <v>5</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>12</v>
@@ -1887,7 +1914,7 @@
         <v>14</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1895,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
@@ -1904,10 +1931,10 @@
         <v>13</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1915,7 +1942,7 @@
         <v>7</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>54</v>
@@ -1927,7 +1954,7 @@
         <v>31</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1935,7 +1962,7 @@
         <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>19</v>
@@ -1947,7 +1974,7 @@
         <v>14</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1955,7 +1982,7 @@
         <v>9</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>12</v>
@@ -1967,7 +1994,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1975,7 +2002,7 @@
         <v>10</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>12</v>
@@ -1987,7 +2014,7 @@
         <v>14</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1995,7 +2022,7 @@
         <v>11</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>19</v>
@@ -2007,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2015,7 +2042,7 @@
         <v>12</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>12</v>
@@ -2027,7 +2054,7 @@
         <v>14</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2035,7 +2062,7 @@
         <v>13</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>54</v>
@@ -2047,7 +2074,7 @@
         <v>14</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>